<commit_message>
added entropy grid visualization
</commit_message>
<xml_diff>
--- a/test_aneupl_file_2.xlsx
+++ b/test_aneupl_file_2.xlsx
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,6 +627,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>